<commit_message>
Competed Machine Learning Algo using Python
</commit_message>
<xml_diff>
--- a/Jigsaw_Progress.xlsx
+++ b/Jigsaw_Progress.xlsx
@@ -13,10 +13,10 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1557592679" val="945" rev="123" rev64="64" revOS="1"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1557592679" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1557592679"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1557592679"/>
+      <pm:revision xmlns:pm="smNativeData" day="1557592799" val="945" rev="123" rev64="64" revOS="1"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1557592799" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1557592799"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1557592799"/>
     </ext>
   </extLst>
 </workbook>
@@ -107,7 +107,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1557592679" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557592799" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -122,7 +122,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1557592679" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1557592799" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -144,7 +144,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1557592679" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557592799" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -155,7 +155,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1557592679" type="1" fgLvl="60" fgClr="004472C4" bgLvl="100" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1557592799" type="1" fgLvl="60" fgClr="004472C4" bgLvl="100" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -177,7 +177,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1557592679"/>
+          <pm:border xmlns:pm="smNativeData" id="1557592799"/>
         </ext>
       </extLst>
     </border>
@@ -196,7 +196,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1557592679"/>
+          <pm:border xmlns:pm="smNativeData" id="1557592799"/>
         </ext>
       </extLst>
     </border>
@@ -215,7 +215,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1557592679"/>
+          <pm:border xmlns:pm="smNativeData" id="1557592799"/>
         </ext>
       </extLst>
     </border>
@@ -242,10 +242,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1557592679" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1557592799" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1557592679" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1557592799" count="1">
         <pm:color name="Color 24" rgb="4472C4"/>
       </pm:colors>
     </ext>
@@ -483,12 +483,12 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="9.666667" customWidth="1"/>
+    <col min="1" max="1" width="12.774775" customWidth="1"/>
     <col min="2" max="2" width="49.729730" customWidth="1"/>
     <col min="3" max="7" width="10.477477" customWidth="1"/>
     <col min="8" max="8" width="21.153153" customWidth="1"/>
@@ -808,7 +808,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5BBE53AE-D40B-F9AB-D911-C30D9AFC1D53}</x14:id>
+          <x14:id>{3C115CD0-EFF9-EE54-CD89-897EEE6E7677}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -816,7 +816,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1557592679" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1557592799" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -825,8 +825,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1557592679" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1557592679" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1557592799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1557592799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -834,7 +834,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5BBE53AE-D40B-F9AB-D911-C30D9AFC1D53}">
+          <x14:cfRule type="dataBar" id="{3C115CD0-EFF9-EE54-CD89-897EEE6E7677}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -849,7 +849,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1557592679" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1557592799" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>